<commit_message>
Code quality imporvement - refactor parts var names , file names to suit for standard. - add requirements.txt - add [WIP] solo_participate support.
</commit_message>
<xml_diff>
--- a/sheets/mappools.xlsx
+++ b/sheets/mappools.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectData\PythonProject\Wikipedia_Edithelper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectData\PythonProject\LiquipediaOsuContributeHelper\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1707F30E-EDAF-46F7-9DAF-6A20686A6611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4850DAA-CD79-475A-8FC9-CC86B3381075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="1950" windowWidth="22160" windowHeight="11470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10400" yWindow="1340" windowWidth="22160" windowHeight="11470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
   <si>
     <t>BID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -134,21 +134,24 @@
     <t>SV2</t>
   </si>
   <si>
-    <t>TB</t>
-  </si>
-  <si>
     <t>SV</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4185651</t>
+    <t>TB1</t>
+  </si>
+  <si>
+    <t>RC7</t>
+  </si>
+  <si>
+    <t>LN4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,10 +199,21 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FFBFA1D8"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -207,10 +221,30 @@
       <color theme="10"/>
       <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFC38AF9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFC38AF9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,42 +265,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF220E38"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF1450B8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF277C4F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5C400"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9E1E1A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD58EFF"/>
+        <fgColor rgb="FF201037"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -296,110 +300,69 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
         <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color rgb="FF6E2B00"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF277C4F"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF58110E"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF58110E"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF277C4F"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF58110E"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF58110E"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF58110E"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFC000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF9E1E1A"/>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFFFC000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF9E1E1A"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF9E1E1A"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF9E1E1A"/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color rgb="FFB46001"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color rgb="FF6E2B00"/>
+      <bottom style="mediumDashed">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color rgb="FF9E1E1A"/>
+      <right style="thick">
+        <color rgb="FF000000"/>
       </right>
-      <top style="medium">
-        <color rgb="FF6E2B00"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF6E2B00"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFB46001"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF6E2B00"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF6E2B00"/>
+      <top/>
+      <bottom style="mediumDashed">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -415,46 +378,46 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="常规 2" xfId="2" xr:uid="{D0556C1D-685F-4F4E-9C60-57050088362B}"/>
+    <cellStyle name="常规 3" xfId="1" xr:uid="{1D92C41B-EC96-4A6F-8427-9AE9C301BD49}"/>
+    <cellStyle name="超链接 2" xfId="3" xr:uid="{EE404957-4456-4690-BCCE-6F8463882C84}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1793,22 +1756,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C2" sqref="C2:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1816,188 +1779,194 @@
       <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="8">
-        <v>4376111</v>
+      <c r="C2" s="7">
+        <v>3763263</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="8">
-        <v>4373684</v>
+      <c r="C3" s="7">
+        <v>3671281</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="8">
-        <v>4373833</v>
+      <c r="C4" s="7">
+        <v>1762209</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="8">
-        <v>4347612</v>
+      <c r="C5" s="7">
+        <v>3756153</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="8">
-        <v>4376216</v>
+      <c r="C6" s="7">
+        <v>3513548</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="8">
-        <v>4375874</v>
+      <c r="C7" s="7">
+        <v>3783809</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="9">
+        <v>3331564</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="9">
-        <v>3402883</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>35</v>
+      <c r="C9" s="13">
+        <v>3793096</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="7">
+        <v>3595933</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="11">
-        <v>4226199</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="C11" s="9">
+        <v>3790784</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="12">
-        <v>4365527</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="C12" s="7">
+        <v>3792661</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="13">
-        <v>3456771</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="C13" s="7">
+        <v>3629447</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B14" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="14">
-        <v>4368219</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="C14" s="7">
+        <v>3792636</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="14">
+        <v>3592063</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="7">
+        <v>3793332</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="9">
+        <v>3793380</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="15">
-        <v>4376223</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="15">
-        <v>4363160</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="16">
-        <v>4249742</v>
-      </c>
-    </row>
+      <c r="C18" s="16">
+        <v>3793375</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" location="mania/4376111" display="https://osu.ppy.sh/beatmapsets/2088245 - mania/4376111" xr:uid="{3F6B575F-7BEC-4602-8737-46B3032E8192}"/>
-    <hyperlink ref="C3" r:id="rId2" location="mania/4373684" display="https://osu.ppy.sh/beatmapsets/2087230 - mania/4373684" xr:uid="{3AE11A20-F741-4BC6-96D8-7D247F7D7CDA}"/>
-    <hyperlink ref="C4" r:id="rId3" location="mania/4373833" display="https://osu.ppy.sh/beatmapsets/2087268 - mania/4373833" xr:uid="{9961B2ED-D95F-4C81-9CBB-0489CA8EDFD3}"/>
-    <hyperlink ref="C5" r:id="rId4" location="mania/4347612" display="https://osu.ppy.sh/beatmapsets/2076495 - mania/4347612" xr:uid="{79DE37FC-5898-463B-911A-DCEC4BA289B4}"/>
-    <hyperlink ref="C6" r:id="rId5" location="mania/4376216" display="https://osu.ppy.sh/beatmapsets/2088296 - mania/4376216" xr:uid="{34FBE4C8-9D93-41F3-8F0F-BEA09F4BAB5E}"/>
-    <hyperlink ref="C7" r:id="rId6" location="mania/4375874" display="https://osu.ppy.sh/beatmapsets/1951169 - mania/4375874" xr:uid="{A521ACA4-EBE7-4263-85F1-94C858DF8BA2}"/>
-    <hyperlink ref="C8" r:id="rId7" location="mania/3402883" display="https://osu.ppy.sh/beatmapsets/1666577 - mania/3402883" xr:uid="{4C1DCA6B-04F0-409A-A66F-D3F5C462EB22}"/>
-    <hyperlink ref="C9" r:id="rId8" location="mania/4185651" display="https://osu.ppy.sh/beatmapsets/2011447 - mania/4185651" xr:uid="{7D8291C6-6B91-4E1A-9B22-CFBA229FD1A1}"/>
-    <hyperlink ref="C10" r:id="rId9" location="mania/4226199" display="https://osu.ppy.sh/beatmapsets/2028112 - mania/4226199" xr:uid="{FD57EBD7-9802-48E7-8A29-2D726B5060CB}"/>
-    <hyperlink ref="C11" r:id="rId10" location="mania/4365527" display="https://osu.ppy.sh/beatmapsets/2084162 - mania/4365527" xr:uid="{EB6AFDF3-18C9-41F1-933A-4A09FB9255A6}"/>
-    <hyperlink ref="C12" r:id="rId11" location="mania/3456771" display="https://osu.ppy.sh/beatmapsets/1691684 - mania/3456771" xr:uid="{9D00E05C-CC41-484D-9B61-02C256C19733}"/>
-    <hyperlink ref="C13" r:id="rId12" location="mania/4368219" display="https://osu.ppy.sh/beatmapsets/2085182 - mania/4368219" xr:uid="{C34EFE39-3884-4DA8-86E1-70B0F28519C5}"/>
-    <hyperlink ref="C14" r:id="rId13" location="mania/4376223" display="https://osu.ppy.sh/beatmapsets/1399179 - mania/4376223" xr:uid="{E62A9510-A7EA-44A4-8517-F1E5BA380752}"/>
-    <hyperlink ref="C15" r:id="rId14" location="mania/4363160" display="https://osu.ppy.sh/beatmapsets/1106399 - mania/4363160" xr:uid="{9D6418B0-C9FF-4250-A492-3DA6D7B7FB3D}"/>
-    <hyperlink ref="C16" r:id="rId15" location="mania/4249742" display="https://osu.ppy.sh/beatmapsets/2037591 - mania/4249742" xr:uid="{DDACDCD4-89B6-4FBC-AAAF-D4343719E9D3}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2012,11 +1981,11 @@
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
+      <c r="A2" s="5"/>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>